<commit_message>
the algorithm now reads the configuration files
</commit_message>
<xml_diff>
--- a/layout/traffic_lights_file.xlsx
+++ b/layout/traffic_lights_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unisabanaedu-my.sharepoint.com/personal/miguelurla_unisabana_edu_co/Documents/GitHub/BRT_C_MEGABUS/layout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="11_F25DC773A252ABDACC104809319B61525BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88325DCA-C074-435F-A3B2-F98A5CA849F4}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_F25DC773A252ABDACC104809319B61525BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{290E44C4-A6BE-4E73-930C-82372064517F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>direction</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>10: 0 - 0 - 0 - 0</t>
+  </si>
+  <si>
+    <t>offset</t>
   </si>
 </sst>
 </file>
@@ -426,20 +429,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="21.42578125" style="1" customWidth="1"/>
-    <col min="4" max="7" width="20.5703125" style="1" customWidth="1"/>
-    <col min="8" max="14" width="20.5703125" customWidth="1"/>
+    <col min="1" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="8" width="20.5703125" style="1" customWidth="1"/>
+    <col min="9" max="15" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -450,40 +453,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -493,17 +499,20 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -513,10 +522,13 @@
       <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>